<commit_message>
Refactored xlsx writer to write any data
</commit_message>
<xml_diff>
--- a/experiments/Expenses01.xlsx
+++ b/experiments/Expenses01.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>EXPENSE</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
   <si>
     <t>Rent</t>
   </si>
@@ -28,7 +34,7 @@
     <t>Gym</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -360,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -370,40 +376,48 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>1000</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>300</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <f>SUM(B1:B4)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>SUM(B2:B5)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>